<commit_message>
Alle Resultate der einzelnen Berechnungen in einer Datei gesichert, da die Daten für die Berechnung nicht zugänglich sind, kleine textliche Änderung in tabPFN_Grade_2
</commit_message>
<xml_diff>
--- a/AI_Auswirkung_S9/Ergebnisse_Vorhersagen.xlsx
+++ b/AI_Auswirkung_S9/Ergebnisse_Vorhersagen.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e194e86fb03a035a/Dokumente/Studium/7. Semester/Artifical Intelligence/Einzelprojekt/AI_Project_01/AI_Auswirkung_S9/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47B92855-C950-47E1-B21C-FB12152876DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="76" documentId="8_{47B92855-C950-47E1-B21C-FB12152876DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47FEEAE7-9821-4B1B-8DBB-17F30900DE4E}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{D67233DF-0AD8-435C-8C88-9440A3C195B2}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{D67233DF-0AD8-435C-8C88-9440A3C195B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Grade_1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="19">
   <si>
     <t>Zeitfenster</t>
   </si>
@@ -67,12 +67,6 @@
   </si>
   <si>
     <t>Verspätung S9</t>
-  </si>
-  <si>
-    <t>Spaltenbeschriftungen</t>
-  </si>
-  <si>
-    <t>Zeilenbeschriftungen</t>
   </si>
   <si>
     <t>Mittelwert von vorhergesagte Grade 1 Verspätung</t>
@@ -102,14 +96,17 @@
     <t>vorhergesagte Verspätung der Grade 2 Züge</t>
   </si>
   <si>
-    <t>Mittelwert von vorhergesagte Verspätung der Grade 2 Züge</t>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Mittelwert von vorhergesagte Grade 2 Verspätung</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,6 +117,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -161,24 +165,3891 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" pivotButton="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" pivotButton="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="204">
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.00000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000000000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -669,19 +4540,19 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A7788ABE-FCE0-4437-97D0-A328B1E6D71E}" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" grandTotalCaption="Mittelwert von vorhergesagte Grade 1 Verspätung" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" compact="0" compactData="0" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A7788ABE-FCE0-4437-97D0-A328B1E6D71E}" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" grandTotalCaption="Mittelwert von vorhergesagte Grade 1 Verspätung" updatedVersion="8" minRefreshableVersion="3" showDrill="0" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A3:G9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
       <items count="5">
+        <item x="0"/>
+        <item x="1"/>
         <item x="2"/>
-        <item x="0"/>
         <item x="3"/>
-        <item x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisCol" compact="0" outline="0" showAll="0">
+    <pivotField name="Verspätung S9 in s" axis="axisCol" compact="0" outline="0" showAll="0">
       <items count="7">
         <item x="0"/>
         <item x="1"/>
@@ -738,40 +4609,72 @@
     </i>
   </colItems>
   <dataFields count="1">
-    <dataField name="Mittelwert von vorhergesagte Grade 1 Verspätung" fld="2" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name=" " fld="2" subtotal="average" baseField="0" baseItem="0"/>
   </dataFields>
-  <formats count="7">
-    <format dxfId="6">
+  <formats count="10">
+    <format dxfId="31">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="5">
+    <format dxfId="32">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="4">
+    <format dxfId="33">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="3">
+    <format dxfId="34">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="2">
+    <format dxfId="35">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="36">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="0">
+    <format dxfId="37">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
+    <format dxfId="38">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
+    </format>
+    <format dxfId="39">
+      <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="40">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="0" selected="0"/>
+        </references>
+      </pivotArea>
+    </format>
   </formats>
-  <pivotTableStyleInfo name="PivotStyleLight19" showRowHeaders="0" showColHeaders="1" showRowStripes="1" showColStripes="0" showLastColumn="1"/>
+  <conditionalFormats count="1">
+    <conditionalFormat priority="1">
+      <pivotAreas count="1">
+        <pivotArea type="data" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="0" count="4" selected="0">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+  </conditionalFormats>
+  <pivotTableStyleInfo name="PivotStyleLight15" showRowHeaders="0" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
@@ -784,30 +4687,28 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{940BBEE8-CF3F-4E92-996F-794635AF96EB}" name="PivotTable2" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" grandTotalCaption="Mittelwert von vorhergesagte Verspätung der Grade 2 Züge" showMissing="0" updatedVersion="8" minRefreshableVersion="3" showDrill="0" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{940BBEE8-CF3F-4E92-996F-794635AF96EB}" name="PivotTable2" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" grandTotalCaption="Mittelwert von vorhergesagte Grade 2 Verspätung" showMissing="0" updatedVersion="8" minRefreshableVersion="3" showDrill="0" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:G9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="5">
+    <pivotField axis="axisRow" compact="0" outline="0" subtotalTop="0" showAll="0" defaultSubtotal="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
         <item x="2"/>
-        <item x="0"/>
         <item x="3"/>
-        <item x="1"/>
-        <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="7">
+    <pivotField axis="axisCol" compact="0" outline="0" subtotalTop="0" showAll="0" defaultSubtotal="0">
+      <items count="6">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
         <item x="3"/>
         <item x="4"/>
         <item x="5"/>
-        <item t="default"/>
       </items>
     </pivotField>
-    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" compact="0" outline="0" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
   <rowFields count="1">
     <field x="0"/>
@@ -853,15 +4754,74 @@
     </i>
   </colItems>
   <dataFields count="1">
-    <dataField name="Mittelwert von vorhergesagte Verspätung der Grade 2 Züge" fld="2" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name=" " fld="2" subtotal="average" baseField="0" baseItem="0" numFmtId="2"/>
   </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="0" showColHeaders="1" showRowStripes="1" showColStripes="0" showLastColumn="1"/>
+  <formats count="7">
+    <format dxfId="136">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="137">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="138">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="139">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="140">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="51">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
+    </format>
+    <format dxfId="1">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <conditionalFormats count="2">
+    <conditionalFormat priority="2">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="0" count="4">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="1">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="0" count="4">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+  </conditionalFormats>
+  <pivotTableStyleInfo name="PivotStyleLight15" showRowHeaders="0" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
     </ext>
     <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
     </ext>
   </extLst>
 </pivotTableDefinition>
@@ -1186,7 +5146,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0C340B7-7966-4018-BD52-3FB2D0957247}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
@@ -1523,169 +5483,182 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C67BCE68-1EB6-47C8-8BC2-3A7BB814FBC8}">
   <dimension ref="A3:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="41.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="5">
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
         <v>60</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="2">
         <v>120</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="2">
         <v>180</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="2">
         <v>300</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="2">
         <v>600</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5">
+        <v>14.312882</v>
+      </c>
+      <c r="C5" s="5">
+        <v>13.002889</v>
+      </c>
+      <c r="D5" s="5">
+        <v>21.809360999999999</v>
+      </c>
+      <c r="E5" s="5">
+        <v>35.431896000000002</v>
+      </c>
+      <c r="F5" s="5">
+        <v>51.843966999999999</v>
+      </c>
+      <c r="G5" s="5">
+        <v>37.698295999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5">
+        <v>4.1598860000000002</v>
+      </c>
+      <c r="C6" s="5">
+        <v>6.6476949999999997</v>
+      </c>
+      <c r="D6" s="5">
+        <v>18.620359000000001</v>
+      </c>
+      <c r="E6" s="5">
+        <v>30.057154000000001</v>
+      </c>
+      <c r="F6" s="5">
+        <v>24.711293999999999</v>
+      </c>
+      <c r="G6" s="5">
+        <v>14.135835</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B7" s="5">
         <v>10.080651</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C7" s="5">
         <v>18.849886000000001</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D7" s="5">
         <v>26.182003000000002</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E7" s="5">
         <v>36.585464000000002</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F7" s="5">
         <v>65.209464999999994</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G7" s="5">
         <v>33.643783999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="6">
-        <v>14.312882</v>
-      </c>
-      <c r="C6" s="6">
-        <v>13.002889</v>
-      </c>
-      <c r="D6" s="6">
-        <v>21.809360999999999</v>
-      </c>
-      <c r="E6" s="6">
-        <v>35.431896000000002</v>
-      </c>
-      <c r="F6" s="6">
-        <v>51.843966999999999</v>
-      </c>
-      <c r="G6" s="6">
-        <v>37.698295999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B8" s="5">
         <v>3.8268499999999999</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C8" s="5">
         <v>6.7631170000000003</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D8" s="5">
         <v>20.618378</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E8" s="5">
         <v>30.412936999999999</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F8" s="5">
         <v>49.510035999999999</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G8" s="5">
         <v>28.170864000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="6">
-        <v>4.1598860000000002</v>
-      </c>
-      <c r="C8" s="6">
-        <v>6.6476949999999997</v>
-      </c>
-      <c r="D8" s="6">
-        <v>18.620359000000001</v>
-      </c>
-      <c r="E8" s="6">
-        <v>30.057154000000001</v>
-      </c>
-      <c r="F8" s="6">
-        <v>24.711293999999999</v>
-      </c>
-      <c r="G8" s="6">
-        <v>14.135835</v>
-      </c>
-    </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="6">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5">
         <v>8.0950672499999996</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>11.31589675</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>21.807525250000005</v>
       </c>
-      <c r="E9" s="6">
-        <v>33.121862749999998</v>
-      </c>
-      <c r="F9" s="6">
+      <c r="E9" s="5">
+        <v>33.121862750000005</v>
+      </c>
+      <c r="F9" s="5">
         <v>47.818690500000002</v>
       </c>
-      <c r="G9" s="6">
-        <v>28.412194750000001</v>
+      <c r="G9" s="5">
+        <v>28.412194749999998</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting pivot="1" sqref="B5:G8">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="9" tint="0.79998168889431442"/>
+        <color theme="5" tint="0.39997558519241921"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1707,31 +5680,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="E1" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="E1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -1859,10 +5832,10 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="7"/>
+      <c r="A11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="3"/>
       <c r="E11" t="s">
         <v>4</v>
       </c>
@@ -1875,10 +5848,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E12" t="s">
         <v>4</v>
@@ -2016,7 +5989,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E21" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -2027,7 +6000,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E22" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F22">
         <v>60</v>
@@ -2038,7 +6011,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E23" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F23">
         <v>120</v>
@@ -2049,7 +6022,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E24" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F24">
         <v>180</v>
@@ -2060,7 +6033,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F25">
         <v>300</v>
@@ -2071,7 +6044,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F26">
         <v>600</v>
@@ -2095,166 +6068,194 @@
   <dimension ref="A3:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="49.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="4" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4">
         <v>0</v>
       </c>
-      <c r="C4">
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
         <v>60</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>120</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>180</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <v>300</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="2">
         <v>600</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="3">
-        <v>6.1251759999999997</v>
-      </c>
-      <c r="C5" s="3">
-        <v>6.6681879999999998</v>
-      </c>
-      <c r="D5" s="3">
-        <v>7.8745419999999999</v>
-      </c>
-      <c r="E5" s="3">
-        <v>8.1919760000000004</v>
-      </c>
-      <c r="F5" s="3">
-        <v>8.4816210000000005</v>
-      </c>
-      <c r="G5" s="3">
-        <v>9.6098999999999997</v>
+        <v>3</v>
+      </c>
+      <c r="B5" s="5">
+        <v>7.4401279999999996</v>
+      </c>
+      <c r="C5" s="5">
+        <v>9.8601759999999992</v>
+      </c>
+      <c r="D5" s="5">
+        <v>11.60248</v>
+      </c>
+      <c r="E5" s="5">
+        <v>13.062037999999999</v>
+      </c>
+      <c r="F5" s="5">
+        <v>14.796046</v>
+      </c>
+      <c r="G5" s="5">
+        <v>16.227029999999999</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="3">
-        <v>7.4401279999999996</v>
-      </c>
-      <c r="C6" s="3">
-        <v>9.8601759999999992</v>
-      </c>
-      <c r="D6" s="3">
-        <v>11.60248</v>
-      </c>
-      <c r="E6" s="3">
-        <v>13.062037999999999</v>
-      </c>
-      <c r="F6" s="3">
-        <v>14.796046</v>
-      </c>
-      <c r="G6" s="3">
-        <v>16.227029999999999</v>
+        <v>4</v>
+      </c>
+      <c r="B6" s="5">
+        <v>4.7691949999999999</v>
+      </c>
+      <c r="C6" s="5">
+        <v>5.3617939999999997</v>
+      </c>
+      <c r="D6" s="5">
+        <v>6.5025769999999996</v>
+      </c>
+      <c r="E6" s="5">
+        <v>6.8989700000000003</v>
+      </c>
+      <c r="F6" s="5">
+        <v>7.5168049999999997</v>
+      </c>
+      <c r="G6" s="5">
+        <v>8.3068749999999998</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="3">
-        <v>5.8949059999999998</v>
-      </c>
-      <c r="C7" s="3">
-        <v>7.503533</v>
-      </c>
-      <c r="D7" s="3">
-        <v>9.5054400000000001</v>
-      </c>
-      <c r="E7" s="3">
-        <v>10.201204000000001</v>
-      </c>
-      <c r="F7" s="3">
-        <v>10.628653</v>
-      </c>
-      <c r="G7" s="3">
-        <v>12.134790000000001</v>
+        <v>5</v>
+      </c>
+      <c r="B7" s="5">
+        <v>6.1251759999999997</v>
+      </c>
+      <c r="C7" s="5">
+        <v>6.6681879999999998</v>
+      </c>
+      <c r="D7" s="5">
+        <v>7.8745419999999999</v>
+      </c>
+      <c r="E7" s="5">
+        <v>8.1919760000000004</v>
+      </c>
+      <c r="F7" s="5">
+        <v>8.4816210000000005</v>
+      </c>
+      <c r="G7" s="5">
+        <v>9.6098999999999997</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="3">
-        <v>4.7691949999999999</v>
-      </c>
-      <c r="C8" s="3">
-        <v>5.3617939999999997</v>
-      </c>
-      <c r="D8" s="3">
-        <v>6.5025769999999996</v>
-      </c>
-      <c r="E8" s="3">
-        <v>6.8989700000000003</v>
-      </c>
-      <c r="F8" s="3">
-        <v>7.5168049999999997</v>
-      </c>
-      <c r="G8" s="3">
-        <v>8.3068749999999998</v>
+        <v>15</v>
+      </c>
+      <c r="B8" s="5">
+        <v>5.8949059999999998</v>
+      </c>
+      <c r="C8" s="5">
+        <v>7.503533</v>
+      </c>
+      <c r="D8" s="5">
+        <v>9.5054400000000001</v>
+      </c>
+      <c r="E8" s="5">
+        <v>10.201204000000001</v>
+      </c>
+      <c r="F8" s="5">
+        <v>10.628653</v>
+      </c>
+      <c r="G8" s="5">
+        <v>12.134790000000001</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="3">
+        <v>18</v>
+      </c>
+      <c r="B9" s="5">
         <v>6.05735125</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="5">
         <v>7.3484227500000001</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="5">
         <v>8.8712597500000001</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="5">
         <v>9.5885470000000002</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="5">
         <v>10.35578125</v>
       </c>
-      <c r="G9" s="3">
-        <v>11.569648749999999</v>
+      <c r="G9" s="5">
+        <v>11.569648750000001</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting pivot="1" sqref="B5:G8">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting pivot="1" sqref="B5:G8">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="9" tint="0.79998168889431442"/>
+        <color theme="5" tint="0.39997558519241921"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>